<commit_message>
update experimental results for Varcop
</commit_message>
<xml_diff>
--- a/experiment_results/DataV2_Results/ExamDB/DISABLE_NORMALIZATION/AGGREGATION_ARITHMETIC_MEAN/4wise/1Bug.xlsx
+++ b/experiment_results/DataV2_Results/ExamDB/DISABLE_NORMALIZATION/AGGREGATION_ARITHMETIC_MEAN/4wise/1Bug.xlsx
@@ -873,7 +873,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1209,13 +1209,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -1595,7 +1595,7 @@
         <v>2.390438247011952</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -2786,7 +2786,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -3122,13 +3122,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -3508,7 +3508,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -4699,7 +4699,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -5035,13 +5035,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -5421,7 +5421,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -6612,7 +6612,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -6948,13 +6948,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -7334,7 +7334,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -8525,7 +8525,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -8861,13 +8861,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -9247,7 +9247,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -10438,7 +10438,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -10774,13 +10774,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -11160,7 +11160,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -12351,7 +12351,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -12687,13 +12687,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -13073,7 +13073,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -14264,7 +14264,7 @@
         <v>3.187250996015936</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>14</v>
@@ -14600,13 +14600,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>1.593625498007968</v>
+        <v>3.98406374501992</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -14986,7 +14986,7 @@
         <v>3.585657370517929</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>14</v>
@@ -16177,7 +16177,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -16513,13 +16513,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>10.35856573705179</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>26</v>
@@ -16899,7 +16899,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -18090,7 +18090,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -18426,13 +18426,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -18812,7 +18812,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -20003,7 +20003,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -20339,13 +20339,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -20725,7 +20725,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -21916,7 +21916,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -22252,13 +22252,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -22638,7 +22638,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -23829,7 +23829,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -24165,13 +24165,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>10.35856573705179</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>26</v>
@@ -24551,7 +24551,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -25742,7 +25742,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -26078,13 +26078,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>37.84860557768924</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>95</v>
@@ -26464,7 +26464,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -27655,7 +27655,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -27991,13 +27991,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>10.35856573705179</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>26</v>
@@ -28377,7 +28377,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -29568,7 +29568,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -29904,13 +29904,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -30290,7 +30290,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -31481,7 +31481,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -31817,13 +31817,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -32203,7 +32203,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -33394,7 +33394,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -33730,13 +33730,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>10.35856573705179</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>26</v>
@@ -34116,7 +34116,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -35307,7 +35307,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -35643,13 +35643,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -36029,7 +36029,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -37220,7 +37220,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -37556,13 +37556,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -37942,7 +37942,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -39133,7 +39133,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -39469,13 +39469,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -39855,7 +39855,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -41046,7 +41046,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -41382,13 +41382,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -41768,7 +41768,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -42959,7 +42959,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -43295,13 +43295,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -43681,7 +43681,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -44872,7 +44872,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -45208,13 +45208,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -45594,7 +45594,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -46785,7 +46785,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -47121,13 +47121,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -47507,7 +47507,7 @@
         <v>2.390438247011952</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -48698,7 +48698,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -49034,13 +49034,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -49420,7 +49420,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -50611,7 +50611,7 @@
         <v>3.187250996015936</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>14</v>
@@ -50947,13 +50947,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>1.593625498007968</v>
+        <v>3.98406374501992</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -51333,7 +51333,7 @@
         <v>3.585657370517929</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>14</v>
@@ -52524,7 +52524,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -52860,13 +52860,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>10.35856573705179</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>26</v>
@@ -53246,7 +53246,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -54437,7 +54437,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -54773,13 +54773,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>10.35856573705179</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>26</v>
@@ -55159,7 +55159,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -56350,7 +56350,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -56686,13 +56686,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0.796812749003984</v>
+        <v>1.195219123505976</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -57072,7 +57072,7 @@
         <v>1.195219123505976</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24">
         <v>3</v>

</xml_diff>